<commit_message>
Saturation Properties Models from Ammonia and Water trained. All saturation properties models validated
</commit_message>
<xml_diff>
--- a/data/SaturationProperties.xlsx
+++ b/data/SaturationProperties.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iaugu\Google Drive (i121006@dac.unicamp.br)\FEQ100010_Especialização em Engenharia de Processos Químicos\FEQ1002_Relações_Termodinâmicas_Equilíbrio_Fases\feq1002_finalwork\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06465D4-C0EB-4069-817E-7F7CFC8FF12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABADC053-AD52-4445-A56B-28BB985E0903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13935" yWindow="2355" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="methane" sheetId="1" r:id="rId1"/>
     <sheet name="ammonia" sheetId="2" r:id="rId2"/>
+    <sheet name="water" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>t</t>
   </si>
@@ -82,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1242,7 +1244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C0490E-C6B6-4424-A62B-A3CFEF3A5664}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
@@ -2191,4 +2193,1599 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA4BE6F-69CA-40E1-93FE-6032DAF49883}">
+  <dimension ref="A1:F79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>273.16000000000003</v>
+      </c>
+      <c r="B2">
+        <v>6.1200000000000002E-4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1.8019E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.1E-5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>280</v>
+      </c>
+      <c r="B3">
+        <v>9.9200000000000004E-4</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1.8017999999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.51876999999999995</v>
+      </c>
+      <c r="F3">
+        <v>1.8760000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>290</v>
+      </c>
+      <c r="B4">
+        <v>1.92E-3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1.8037999999999998E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.2742</v>
+      </c>
+      <c r="F4">
+        <v>4.5269999999999998E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>3.5370000000000002E-3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1.8079000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.0278999999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.0819999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>310</v>
+      </c>
+      <c r="B6">
+        <v>6.2310000000000004E-3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.8135999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.7810000000000001</v>
+      </c>
+      <c r="F6">
+        <v>9.5510000000000005E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>320</v>
+      </c>
+      <c r="B7">
+        <v>1.0546E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1.8208999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>3.5339999999999998</v>
+      </c>
+      <c r="F7">
+        <v>1.1941E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>330</v>
+      </c>
+      <c r="B8">
+        <v>1.7212999999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1.8294000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>4.2876000000000003</v>
+      </c>
+      <c r="F8">
+        <v>1.426E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>340</v>
+      </c>
+      <c r="B9">
+        <v>2.7188E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1.8391999999999999E-2</v>
+      </c>
+      <c r="E9">
+        <v>5.0419</v>
+      </c>
+      <c r="F9">
+        <v>1.6511000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>350</v>
+      </c>
+      <c r="B10">
+        <v>4.1681999999999997E-2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1.8502000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>5.7972000000000001</v>
+      </c>
+      <c r="F10">
+        <v>1.8700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>360</v>
+      </c>
+      <c r="B11">
+        <v>6.2193999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.8623000000000001E-2</v>
+      </c>
+      <c r="E11">
+        <v>6.5537999999999998</v>
+      </c>
+      <c r="F11">
+        <v>2.0830000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>370</v>
+      </c>
+      <c r="B12">
+        <v>9.0535000000000004E-2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.8754E-2</v>
+      </c>
+      <c r="E12">
+        <v>7.3121</v>
+      </c>
+      <c r="F12">
+        <v>2.2905999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>380</v>
+      </c>
+      <c r="B13">
+        <v>0.12884999999999999</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1.8897000000000001E-2</v>
+      </c>
+      <c r="E13">
+        <v>8.0724999999999998</v>
+      </c>
+      <c r="F13">
+        <v>2.4931999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>390</v>
+      </c>
+      <c r="B14">
+        <v>0.17963999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1.9050999999999998E-2</v>
+      </c>
+      <c r="E14">
+        <v>8.8353999999999999</v>
+      </c>
+      <c r="F14">
+        <v>2.6911000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>400</v>
+      </c>
+      <c r="B15">
+        <v>0.24576999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1.9217000000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>9.6013000000000002</v>
+      </c>
+      <c r="F15">
+        <v>2.8847000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>410</v>
+      </c>
+      <c r="B16">
+        <v>0.33045000000000002</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1.9394000000000002E-2</v>
+      </c>
+      <c r="E16">
+        <v>10.371</v>
+      </c>
+      <c r="F16">
+        <v>3.0742999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>420</v>
+      </c>
+      <c r="B17">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1.9583E-2</v>
+      </c>
+      <c r="E17">
+        <v>11.144</v>
+      </c>
+      <c r="F17">
+        <v>3.2601999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>430</v>
+      </c>
+      <c r="B18">
+        <v>0.57025999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1.9786000000000002E-2</v>
+      </c>
+      <c r="E18">
+        <v>11.923</v>
+      </c>
+      <c r="F18">
+        <v>3.4426999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>440</v>
+      </c>
+      <c r="B19">
+        <v>0.73367000000000004</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2.0003E-2</v>
+      </c>
+      <c r="E19">
+        <v>12.706</v>
+      </c>
+      <c r="F19">
+        <v>3.6221999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>450</v>
+      </c>
+      <c r="B20">
+        <v>0.93220000000000003</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>2.0233999999999999E-2</v>
+      </c>
+      <c r="E20">
+        <v>13.496</v>
+      </c>
+      <c r="F20">
+        <v>3.7988000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>460</v>
+      </c>
+      <c r="B21">
+        <v>1.1709000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2.0482E-2</v>
+      </c>
+      <c r="E21">
+        <v>14.292999999999999</v>
+      </c>
+      <c r="F21">
+        <v>3.9729E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>470</v>
+      </c>
+      <c r="B22">
+        <v>1.4551000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2.0747999999999999E-2</v>
+      </c>
+      <c r="E22">
+        <v>15.098000000000001</v>
+      </c>
+      <c r="F22">
+        <v>4.1447999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>480</v>
+      </c>
+      <c r="B23">
+        <v>1.7905</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>2.1033E-2</v>
+      </c>
+      <c r="E23">
+        <v>15.913</v>
+      </c>
+      <c r="F23">
+        <v>4.3146999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>490</v>
+      </c>
+      <c r="B24">
+        <v>2.1831</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2.1340000000000001E-2</v>
+      </c>
+      <c r="E24">
+        <v>16.736999999999998</v>
+      </c>
+      <c r="F24">
+        <v>4.4830000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>500</v>
+      </c>
+      <c r="B25">
+        <v>2.6392000000000002</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2.1670999999999999E-2</v>
+      </c>
+      <c r="E25">
+        <v>17.573</v>
+      </c>
+      <c r="F25">
+        <v>4.6497999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>510</v>
+      </c>
+      <c r="B26">
+        <v>3.1655000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>2.2030000000000001E-2</v>
+      </c>
+      <c r="E26">
+        <v>18.420999999999999</v>
+      </c>
+      <c r="F26">
+        <v>4.8155999999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>520</v>
+      </c>
+      <c r="B27">
+        <v>3.7690000000000001</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2.2419999999999999E-2</v>
+      </c>
+      <c r="E27">
+        <v>19.285</v>
+      </c>
+      <c r="F27">
+        <v>4.9806999999999997E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>530</v>
+      </c>
+      <c r="B28">
+        <v>4.4569000000000001</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>2.2846999999999999E-2</v>
+      </c>
+      <c r="E28">
+        <v>20.164999999999999</v>
+      </c>
+      <c r="F28">
+        <v>5.1454E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>540</v>
+      </c>
+      <c r="B29">
+        <v>5.2369000000000003</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>2.3316E-2</v>
+      </c>
+      <c r="E29">
+        <v>21.065000000000001</v>
+      </c>
+      <c r="F29">
+        <v>5.3102000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>550</v>
+      </c>
+      <c r="B30">
+        <v>6.1172000000000004</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>2.3836E-2</v>
+      </c>
+      <c r="E30">
+        <v>21.986999999999998</v>
+      </c>
+      <c r="F30">
+        <v>5.4755999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>560</v>
+      </c>
+      <c r="B31">
+        <v>7.1062000000000003</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2.4417000000000001E-2</v>
+      </c>
+      <c r="E31">
+        <v>22.934999999999999</v>
+      </c>
+      <c r="F31">
+        <v>5.6422E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>570</v>
+      </c>
+      <c r="B32">
+        <v>8.2132000000000005</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2.5072000000000001E-2</v>
+      </c>
+      <c r="E32">
+        <v>23.914999999999999</v>
+      </c>
+      <c r="F32">
+        <v>5.8105999999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>580</v>
+      </c>
+      <c r="B33">
+        <v>9.4480000000000004</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>2.5822999999999999E-2</v>
+      </c>
+      <c r="E33">
+        <v>24.931999999999999</v>
+      </c>
+      <c r="F33">
+        <v>5.9820999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>590</v>
+      </c>
+      <c r="B34">
+        <v>10.821</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>2.6698E-2</v>
+      </c>
+      <c r="E34">
+        <v>25.995999999999999</v>
+      </c>
+      <c r="F34">
+        <v>6.1577E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>600</v>
+      </c>
+      <c r="B35">
+        <v>12.345000000000001</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>2.7740999999999998E-2</v>
+      </c>
+      <c r="E35">
+        <v>27.119</v>
+      </c>
+      <c r="F35">
+        <v>6.3395999999999994E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>610</v>
+      </c>
+      <c r="B36">
+        <v>14.032999999999999</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>2.9026E-2</v>
+      </c>
+      <c r="E36">
+        <v>28.324000000000002</v>
+      </c>
+      <c r="F36">
+        <v>6.5309000000000006E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>620</v>
+      </c>
+      <c r="B37">
+        <v>15.901</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>3.0696999999999999E-2</v>
+      </c>
+      <c r="E37">
+        <v>29.648</v>
+      </c>
+      <c r="F37">
+        <v>6.7371E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>630</v>
+      </c>
+      <c r="B38">
+        <v>17.969000000000001</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>3.3100999999999998E-2</v>
+      </c>
+      <c r="E38">
+        <v>31.18</v>
+      </c>
+      <c r="F38">
+        <v>6.9714999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>640</v>
+      </c>
+      <c r="B39">
+        <v>20.265000000000001</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>3.7413000000000002E-2</v>
+      </c>
+      <c r="E39">
+        <v>33.18</v>
+      </c>
+      <c r="F39">
+        <v>7.2736999999999996E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>647.1</v>
+      </c>
+      <c r="B40">
+        <v>22.064</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>5.5947999999999998E-2</v>
+      </c>
+      <c r="E40">
+        <v>37.548000000000002</v>
+      </c>
+      <c r="F40">
+        <v>7.9393000000000005E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>273.16000000000003</v>
+      </c>
+      <c r="B41">
+        <v>6.1200000000000002E-4</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>3711</v>
+      </c>
+      <c r="E41">
+        <v>45.055</v>
+      </c>
+      <c r="F41">
+        <v>0.16494</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>280</v>
+      </c>
+      <c r="B42">
+        <v>9.9200000000000004E-4</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2345.4</v>
+      </c>
+      <c r="E42">
+        <v>45.28</v>
+      </c>
+      <c r="F42">
+        <v>0.16173999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>290</v>
+      </c>
+      <c r="B43">
+        <v>1.92E-3</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1254.3</v>
+      </c>
+      <c r="E43">
+        <v>45.609000000000002</v>
+      </c>
+      <c r="F43">
+        <v>0.15740999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>300</v>
+      </c>
+      <c r="B44">
+        <v>3.5370000000000002E-3</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>704.01</v>
+      </c>
+      <c r="E44">
+        <v>45.936</v>
+      </c>
+      <c r="F44">
+        <v>0.15343999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>310</v>
+      </c>
+      <c r="B45">
+        <v>6.2310000000000004E-3</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>412.6</v>
+      </c>
+      <c r="E45">
+        <v>46.261000000000003</v>
+      </c>
+      <c r="F45">
+        <v>0.14981</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>320</v>
+      </c>
+      <c r="B46">
+        <v>1.0546E-2</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>251.39</v>
+      </c>
+      <c r="E46">
+        <v>46.582000000000001</v>
+      </c>
+      <c r="F46">
+        <v>0.14646999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>330</v>
+      </c>
+      <c r="B47">
+        <v>1.7212999999999999E-2</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>158.62</v>
+      </c>
+      <c r="E47">
+        <v>46.9</v>
+      </c>
+      <c r="F47">
+        <v>0.14338999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>340</v>
+      </c>
+      <c r="B48">
+        <v>2.7188E-2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>103.3</v>
+      </c>
+      <c r="E48">
+        <v>47.212000000000003</v>
+      </c>
+      <c r="F48">
+        <v>0.14054</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>350</v>
+      </c>
+      <c r="B49">
+        <v>4.1681999999999997E-2</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>69.212999999999994</v>
+      </c>
+      <c r="E49">
+        <v>47.518999999999998</v>
+      </c>
+      <c r="F49">
+        <v>0.13791</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>360</v>
+      </c>
+      <c r="B50">
+        <v>6.2193999999999999E-2</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>47.585999999999999</v>
+      </c>
+      <c r="E50">
+        <v>47.819000000000003</v>
+      </c>
+      <c r="F50">
+        <v>0.13546</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>370</v>
+      </c>
+      <c r="B51">
+        <v>9.0535000000000004E-2</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>33.491</v>
+      </c>
+      <c r="E51">
+        <v>48.110999999999997</v>
+      </c>
+      <c r="F51">
+        <v>0.13317000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>380</v>
+      </c>
+      <c r="B52">
+        <v>0.12884999999999999</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>24.074999999999999</v>
+      </c>
+      <c r="E52">
+        <v>48.393000000000001</v>
+      </c>
+      <c r="F52">
+        <v>0.13103999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>390</v>
+      </c>
+      <c r="B53">
+        <v>0.17963999999999999</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>17.641999999999999</v>
+      </c>
+      <c r="E53">
+        <v>48.664999999999999</v>
+      </c>
+      <c r="F53">
+        <v>0.12903999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>400</v>
+      </c>
+      <c r="B54">
+        <v>0.24576999999999999</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>13.156000000000001</v>
+      </c>
+      <c r="E54">
+        <v>48.923999999999999</v>
+      </c>
+      <c r="F54">
+        <v>0.12715000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>410</v>
+      </c>
+      <c r="B55">
+        <v>0.33045000000000002</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>9.9665999999999997</v>
+      </c>
+      <c r="E55">
+        <v>49.17</v>
+      </c>
+      <c r="F55">
+        <v>0.12537000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>420</v>
+      </c>
+      <c r="B56">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>7.6600999999999999</v>
+      </c>
+      <c r="E56">
+        <v>49.4</v>
+      </c>
+      <c r="F56">
+        <v>0.12368999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>430</v>
+      </c>
+      <c r="B57">
+        <v>0.57025999999999999</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>5.9649000000000001</v>
+      </c>
+      <c r="E57">
+        <v>49.613</v>
+      </c>
+      <c r="F57">
+        <v>0.12207999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>440</v>
+      </c>
+      <c r="B58">
+        <v>0.73367000000000004</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>4.7001999999999997</v>
+      </c>
+      <c r="E58">
+        <v>49.807000000000002</v>
+      </c>
+      <c r="F58">
+        <v>0.12053999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>450</v>
+      </c>
+      <c r="B59">
+        <v>0.93220000000000003</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>3.7437999999999998</v>
+      </c>
+      <c r="E59">
+        <v>49.981999999999999</v>
+      </c>
+      <c r="F59">
+        <v>0.11907</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>460</v>
+      </c>
+      <c r="B60">
+        <v>1.1709000000000001</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>3.0112999999999999</v>
+      </c>
+      <c r="E60">
+        <v>50.134</v>
+      </c>
+      <c r="F60">
+        <v>0.11763999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>470</v>
+      </c>
+      <c r="B61">
+        <v>1.4551000000000001</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>2.4434999999999998</v>
+      </c>
+      <c r="E61">
+        <v>50.262999999999998</v>
+      </c>
+      <c r="F61">
+        <v>0.11627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>480</v>
+      </c>
+      <c r="B62">
+        <v>1.7905</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1.9985999999999999</v>
+      </c>
+      <c r="E62">
+        <v>50.366999999999997</v>
+      </c>
+      <c r="F62">
+        <v>0.11493</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>490</v>
+      </c>
+      <c r="B63">
+        <v>2.1831</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1.6464000000000001</v>
+      </c>
+      <c r="E63">
+        <v>50.442</v>
+      </c>
+      <c r="F63">
+        <v>0.11362</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>500</v>
+      </c>
+      <c r="B64">
+        <v>2.6392000000000002</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1.3649</v>
+      </c>
+      <c r="E64">
+        <v>50.487000000000002</v>
+      </c>
+      <c r="F64">
+        <v>0.11233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>510</v>
+      </c>
+      <c r="B65">
+        <v>3.1655000000000002</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1.1378999999999999</v>
+      </c>
+      <c r="E65">
+        <v>50.5</v>
+      </c>
+      <c r="F65">
+        <v>0.11105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>520</v>
+      </c>
+      <c r="B66">
+        <v>3.7690000000000001</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>0.95318000000000003</v>
+      </c>
+      <c r="E66">
+        <v>50.475000000000001</v>
+      </c>
+      <c r="F66">
+        <v>0.10979</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>530</v>
+      </c>
+      <c r="B67">
+        <v>4.4569000000000001</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>0.80174000000000001</v>
+      </c>
+      <c r="E67">
+        <v>50.411000000000001</v>
+      </c>
+      <c r="F67">
+        <v>0.10852000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>540</v>
+      </c>
+      <c r="B68">
+        <v>5.2369000000000003</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0.67659000000000002</v>
+      </c>
+      <c r="E68">
+        <v>50.302</v>
+      </c>
+      <c r="F68">
+        <v>0.10724</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>550</v>
+      </c>
+      <c r="B69">
+        <v>6.1172000000000004</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0.57238</v>
+      </c>
+      <c r="E69">
+        <v>50.142000000000003</v>
+      </c>
+      <c r="F69">
+        <v>0.10595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>560</v>
+      </c>
+      <c r="B70">
+        <v>7.1062000000000003</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0.48497000000000001</v>
+      </c>
+      <c r="E70">
+        <v>49.924999999999997</v>
+      </c>
+      <c r="F70">
+        <v>0.10462</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>570</v>
+      </c>
+      <c r="B71">
+        <v>8.2132000000000005</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0.41110000000000002</v>
+      </c>
+      <c r="E71">
+        <v>49.640999999999998</v>
+      </c>
+      <c r="F71">
+        <v>0.10324</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>580</v>
+      </c>
+      <c r="B72">
+        <v>9.4480000000000004</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0.34819</v>
+      </c>
+      <c r="E72">
+        <v>49.277999999999999</v>
+      </c>
+      <c r="F72">
+        <v>0.1018</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>590</v>
+      </c>
+      <c r="B73">
+        <v>10.821</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0.29416999999999999</v>
+      </c>
+      <c r="E73">
+        <v>48.819000000000003</v>
+      </c>
+      <c r="F73">
+        <v>0.10026</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>600</v>
+      </c>
+      <c r="B74">
+        <v>12.345000000000001</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0.24732000000000001</v>
+      </c>
+      <c r="E74">
+        <v>48.241999999999997</v>
+      </c>
+      <c r="F74">
+        <v>9.8599999999999993E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>610</v>
+      </c>
+      <c r="B75">
+        <v>14.032999999999999</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="E75">
+        <v>47.506</v>
+      </c>
+      <c r="F75">
+        <v>9.6754999999999994E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>620</v>
+      </c>
+      <c r="B76">
+        <v>15.901</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>0.16946</v>
+      </c>
+      <c r="E76">
+        <v>46.55</v>
+      </c>
+      <c r="F76">
+        <v>9.4631000000000007E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>630</v>
+      </c>
+      <c r="B77">
+        <v>17.969000000000001</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0.13561999999999999</v>
+      </c>
+      <c r="E77">
+        <v>45.238</v>
+      </c>
+      <c r="F77">
+        <v>9.2029E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>640</v>
+      </c>
+      <c r="B78">
+        <v>20.265000000000001</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0.1017</v>
+      </c>
+      <c r="E78">
+        <v>43.155999999999999</v>
+      </c>
+      <c r="F78">
+        <v>8.8324E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>647.1</v>
+      </c>
+      <c r="B79">
+        <v>22.064</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>5.5947999999999998E-2</v>
+      </c>
+      <c r="E79">
+        <v>37.548000000000002</v>
+      </c>
+      <c r="F79">
+        <v>7.9393000000000005E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>